<commit_message>
Fixing excel uploads and memberships
Signed-off-by: mbaskhairounTelus <michael.baskhairoun@telus.com>
</commit_message>
<xml_diff>
--- a/To Add.xlsx
+++ b/To Add.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://proserveit-my.sharepoint.com/personal/mbaskhairoun_linezero_com/Documents/Desktop/Upwork/sgsascouts.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="155" documentId="11_F25DC773A252ABDACC104868095C4B345ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54E13946-82E9-43C6-B04E-FE4D5032ED1D}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="11_F25DC773A252ABDACC104868095C4B345ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{421FF311-02A6-4843-9FFB-6BB790CD7F2B}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,9 +72,6 @@
     <t>Parent Name</t>
   </si>
   <si>
-    <t>Parent Phone</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -334,6 +331,9 @@
   </si>
   <si>
     <t>Filata</t>
+  </si>
+  <si>
+    <t>parent phone</t>
   </si>
 </sst>
 </file>
@@ -767,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,75 +793,75 @@
         <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="C2" s="5">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="C3" s="5">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="C4" s="5">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="C5" s="5">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -869,67 +869,67 @@
         <v>0</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="5">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="C7" s="5">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="C8" s="5">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="5">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -937,38 +937,38 @@
         <v>4</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="5">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="C11" s="5">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>3</v>
@@ -977,78 +977,78 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="C13" s="5">
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="C14" s="5">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="C15" s="5">
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E15" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="C16" s="3">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E16" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1056,16 +1056,16 @@
         <v>7</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="3">
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E17" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1073,33 +1073,33 @@
         <v>7</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" s="3">
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="C19" s="5">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E19" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1107,16 +1107,16 @@
         <v>9</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="5">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E20" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1130,49 +1130,49 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E21" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" s="5">
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E22" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="C23" s="5">
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E23" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>1</v>
@@ -1181,27 +1181,27 @@
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E24" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25" s="5">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E25" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1209,16 +1209,16 @@
         <v>6</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" s="5">
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E26" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1226,72 +1226,72 @@
         <v>2</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C27" s="5">
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E27" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="9" t="s">
-        <v>60</v>
-      </c>
       <c r="C28" s="5">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E28" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>61</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>62</v>
       </c>
       <c r="C29" s="3">
         <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E29" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="C30" s="5">
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E30" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>5</v>
@@ -1300,27 +1300,27 @@
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E31" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B32" s="9" t="s">
-        <v>67</v>
-      </c>
       <c r="C32" s="5">
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E32" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1328,55 +1328,55 @@
         <v>4</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="5">
         <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E33" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="9" t="s">
-        <v>70</v>
-      </c>
       <c r="C34" s="5">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E34" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>72</v>
-      </c>
       <c r="C35" s="11">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E35" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>10</v>
@@ -1385,66 +1385,66 @@
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E36" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="9" t="s">
-        <v>74</v>
-      </c>
       <c r="C37" s="5">
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E37" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C38" s="5">
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E38" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="C39" s="5">
         <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E39" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>8</v>
@@ -1453,49 +1453,49 @@
         <v>4</v>
       </c>
       <c r="D40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E40" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C41" s="11">
         <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E41" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" s="9" t="s">
         <v>80</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>81</v>
       </c>
       <c r="C42" s="5">
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E42" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>1</v>
@@ -1504,27 +1504,27 @@
         <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E43" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C44" s="5">
         <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E44" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1532,50 +1532,50 @@
         <v>0</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C45" s="5">
         <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E45" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B46" s="9" t="s">
-        <v>85</v>
-      </c>
       <c r="C46" s="5">
         <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E46" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="C47" s="5">
         <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E47" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1583,16 +1583,16 @@
         <v>9</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C48" s="5">
         <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E48" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1600,152 +1600,152 @@
         <v>2</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C49" s="3">
         <v>3</v>
       </c>
       <c r="D49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E49" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C50" s="3">
         <v>3</v>
       </c>
       <c r="D50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E50" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="C51" s="3">
         <v>3</v>
       </c>
       <c r="D51" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E51" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="C52" s="3">
         <v>3</v>
       </c>
       <c r="D52" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E52" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C53" s="3">
         <v>3</v>
       </c>
       <c r="D53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E53" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C54" s="3">
         <v>3</v>
       </c>
       <c r="D54" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E54" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="C55" s="3">
         <v>3</v>
       </c>
       <c r="D55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E55" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="C56" s="3">
         <v>3</v>
       </c>
       <c r="D56" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E56" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C57" s="3">
         <v>3</v>
       </c>
       <c r="D57" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E57" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1753,33 +1753,33 @@
         <v>4</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C58" s="3">
         <v>3</v>
       </c>
       <c r="D58" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E58" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="C59" s="3">
         <v>3</v>
       </c>
       <c r="D59" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E59" s="1">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>